<commit_message>
Country-specific electricity and heat price
</commit_message>
<xml_diff>
--- a/Parameters/technology_parameters.xlsx
+++ b/Parameters/technology_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9A8A10-2639-984B-B8E9-6349C1867982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9439714-4816-924C-A763-65DCBB656576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" activeTab="1" xr2:uid="{C2021D4B-F101-9446-A40F-20FC94B0106D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16760" xr2:uid="{C2021D4B-F101-9446-A40F-20FC94B0106D}"/>
   </bookViews>
   <sheets>
     <sheet name="Water" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>CAPEX</t>
   </si>
@@ -80,16 +80,26 @@
   </si>
   <si>
     <t>Road construction allowed</t>
+  </si>
+  <si>
+    <t>Water demand  (L/kg H2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F260B15A-B8F5-44FB-9EF4-FDC040BBCD83}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,6 +490,14 @@
         <v>1.25</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -488,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F43247-4FF6-844F-9F39-98135821A884}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,10 +572,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AA0EAD-92E5-46DC-A6CE-8D3F449C6741}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,33 +590,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>1.2</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>33.33</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>